<commit_message>
Actualizacion de Utilidades y Contingencia Automatica
</commit_message>
<xml_diff>
--- a/uploads/EspecificoCategoria/EspecificoCategoria_relaves.xlsx
+++ b/uploads/EspecificoCategoria/EspecificoCategoria_relaves.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://enami-my.sharepoint.com/personal/pjdiaz_enami_cl/Documents/Escritorio/duplicado relaves/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://enami-my.sharepoint.com/personal/pjdiaz_enami_cl/Documents/Escritorio/Proyecto37/Proyecto16/Proyecto11/proyecto2/uploads/EspecificoCategoria/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_23F921ED90E30811DB2D4C98BDDC611C7D26867C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE22C59D-7D9F-4621-8FD7-89D1138182CE}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_23F921ED90E30811DB2D4C98BDDC611C7D26867C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9378B00-E2C2-48C0-911D-10636F074FB7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="85">
   <si>
     <t>id_categoria</t>
   </si>
@@ -657,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H56"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -693,8 +693,8 @@
       <c r="C2" t="s">
         <v>68</v>
       </c>
-      <c r="D2" t="s">
-        <v>68</v>
+      <c r="D2">
+        <v>100</v>
       </c>
       <c r="E2" t="s">
         <v>80</v>
@@ -713,8 +713,8 @@
       <c r="C3" t="s">
         <v>68</v>
       </c>
-      <c r="D3" t="s">
-        <v>68</v>
+      <c r="D3">
+        <v>100</v>
       </c>
       <c r="E3" t="s">
         <v>81</v>
@@ -733,8 +733,8 @@
       <c r="C4" t="s">
         <v>68</v>
       </c>
-      <c r="D4" t="s">
-        <v>68</v>
+      <c r="D4">
+        <v>100</v>
       </c>
       <c r="E4" t="s">
         <v>82</v>
@@ -753,8 +753,8 @@
       <c r="C5" t="s">
         <v>68</v>
       </c>
-      <c r="D5" t="s">
-        <v>68</v>
+      <c r="D5">
+        <v>100</v>
       </c>
       <c r="E5" t="s">
         <v>80</v>
@@ -773,8 +773,8 @@
       <c r="C6" t="s">
         <v>68</v>
       </c>
-      <c r="D6" t="s">
-        <v>68</v>
+      <c r="D6">
+        <v>100</v>
       </c>
       <c r="E6" t="s">
         <v>81</v>
@@ -793,8 +793,8 @@
       <c r="C7" t="s">
         <v>68</v>
       </c>
-      <c r="D7" t="s">
-        <v>68</v>
+      <c r="D7">
+        <v>100</v>
       </c>
       <c r="E7" t="s">
         <v>81</v>
@@ -813,8 +813,8 @@
       <c r="C8" t="s">
         <v>68</v>
       </c>
-      <c r="D8" t="s">
-        <v>68</v>
+      <c r="D8">
+        <v>100</v>
       </c>
       <c r="E8" t="s">
         <v>80</v>
@@ -833,8 +833,8 @@
       <c r="C9" t="s">
         <v>68</v>
       </c>
-      <c r="D9" t="s">
-        <v>68</v>
+      <c r="D9">
+        <v>100</v>
       </c>
       <c r="E9" t="s">
         <v>83</v>
@@ -853,8 +853,8 @@
       <c r="C10" t="s">
         <v>68</v>
       </c>
-      <c r="D10" t="s">
-        <v>68</v>
+      <c r="D10">
+        <v>100</v>
       </c>
       <c r="E10" t="s">
         <v>81</v>
@@ -873,8 +873,8 @@
       <c r="C11" t="s">
         <v>68</v>
       </c>
-      <c r="D11" t="s">
-        <v>68</v>
+      <c r="D11">
+        <v>100</v>
       </c>
       <c r="E11" t="s">
         <v>82</v>
@@ -893,8 +893,8 @@
       <c r="C12" t="s">
         <v>68</v>
       </c>
-      <c r="D12" t="s">
-        <v>68</v>
+      <c r="D12">
+        <v>100</v>
       </c>
       <c r="E12" t="s">
         <v>82</v>
@@ -913,8 +913,8 @@
       <c r="C13" t="s">
         <v>68</v>
       </c>
-      <c r="D13" t="s">
-        <v>68</v>
+      <c r="D13">
+        <v>100</v>
       </c>
       <c r="E13" t="s">
         <v>84</v>
@@ -933,8 +933,8 @@
       <c r="C14" t="s">
         <v>68</v>
       </c>
-      <c r="D14" t="s">
-        <v>68</v>
+      <c r="D14">
+        <v>100</v>
       </c>
       <c r="E14" t="s">
         <v>84</v>
@@ -953,8 +953,8 @@
       <c r="C15" t="s">
         <v>68</v>
       </c>
-      <c r="D15" t="s">
-        <v>68</v>
+      <c r="D15">
+        <v>100</v>
       </c>
       <c r="E15" t="s">
         <v>81</v>
@@ -973,8 +973,8 @@
       <c r="C16" t="s">
         <v>68</v>
       </c>
-      <c r="D16" t="s">
-        <v>68</v>
+      <c r="D16">
+        <v>100</v>
       </c>
       <c r="E16" t="s">
         <v>69</v>
@@ -993,8 +993,8 @@
       <c r="C17" t="s">
         <v>68</v>
       </c>
-      <c r="D17" t="s">
-        <v>68</v>
+      <c r="D17">
+        <v>100</v>
       </c>
       <c r="E17" t="s">
         <v>77</v>
@@ -1013,8 +1013,8 @@
       <c r="C18" t="s">
         <v>68</v>
       </c>
-      <c r="D18" t="s">
-        <v>68</v>
+      <c r="D18">
+        <v>100</v>
       </c>
       <c r="E18" t="s">
         <v>77</v>
@@ -1033,8 +1033,8 @@
       <c r="C19" t="s">
         <v>69</v>
       </c>
-      <c r="D19" t="s">
-        <v>68</v>
+      <c r="D19">
+        <v>100</v>
       </c>
       <c r="E19" t="s">
         <v>69</v>
@@ -1053,8 +1053,8 @@
       <c r="C20" t="s">
         <v>68</v>
       </c>
-      <c r="D20" t="s">
-        <v>68</v>
+      <c r="D20">
+        <v>100</v>
       </c>
       <c r="E20" t="s">
         <v>82</v>
@@ -1073,8 +1073,8 @@
       <c r="C21" t="s">
         <v>70</v>
       </c>
-      <c r="D21" t="s">
-        <v>68</v>
+      <c r="D21">
+        <v>100</v>
       </c>
       <c r="E21" t="s">
         <v>81</v>
@@ -1093,8 +1093,8 @@
       <c r="C22" t="s">
         <v>71</v>
       </c>
-      <c r="D22" t="s">
-        <v>68</v>
+      <c r="D22">
+        <v>100</v>
       </c>
       <c r="E22" t="s">
         <v>68</v>
@@ -1113,8 +1113,8 @@
       <c r="C23" t="s">
         <v>71</v>
       </c>
-      <c r="D23" t="s">
-        <v>68</v>
+      <c r="D23">
+        <v>100</v>
       </c>
       <c r="E23" t="s">
         <v>68</v>
@@ -1133,8 +1133,8 @@
       <c r="C24" t="s">
         <v>72</v>
       </c>
-      <c r="D24" t="s">
-        <v>68</v>
+      <c r="D24">
+        <v>100</v>
       </c>
       <c r="E24" t="s">
         <v>68</v>
@@ -1153,8 +1153,8 @@
       <c r="C25" t="s">
         <v>73</v>
       </c>
-      <c r="D25" t="s">
-        <v>68</v>
+      <c r="D25">
+        <v>100</v>
       </c>
       <c r="E25" t="s">
         <v>68</v>
@@ -1173,8 +1173,8 @@
       <c r="C26" t="s">
         <v>68</v>
       </c>
-      <c r="D26" t="s">
-        <v>68</v>
+      <c r="D26">
+        <v>100</v>
       </c>
       <c r="E26" t="s">
         <v>82</v>
@@ -1193,8 +1193,8 @@
       <c r="C27" t="s">
         <v>69</v>
       </c>
-      <c r="D27" t="s">
-        <v>68</v>
+      <c r="D27">
+        <v>100</v>
       </c>
       <c r="E27" t="s">
         <v>80</v>
@@ -1213,8 +1213,8 @@
       <c r="C28" t="s">
         <v>68</v>
       </c>
-      <c r="D28" t="s">
-        <v>68</v>
+      <c r="D28">
+        <v>100</v>
       </c>
       <c r="E28" t="s">
         <v>80</v>
@@ -1233,8 +1233,8 @@
       <c r="C29" t="s">
         <v>73</v>
       </c>
-      <c r="D29" t="s">
-        <v>68</v>
+      <c r="D29">
+        <v>100</v>
       </c>
       <c r="E29" t="s">
         <v>80</v>
@@ -1253,8 +1253,8 @@
       <c r="C30" t="s">
         <v>74</v>
       </c>
-      <c r="D30" t="s">
-        <v>68</v>
+      <c r="D30">
+        <v>100</v>
       </c>
       <c r="E30" t="s">
         <v>80</v>
@@ -1273,8 +1273,8 @@
       <c r="C31" t="s">
         <v>68</v>
       </c>
-      <c r="D31" t="s">
-        <v>68</v>
+      <c r="D31">
+        <v>100</v>
       </c>
       <c r="E31" t="s">
         <v>81</v>
@@ -1293,8 +1293,8 @@
       <c r="C32" t="s">
         <v>75</v>
       </c>
-      <c r="D32" t="s">
-        <v>68</v>
+      <c r="D32">
+        <v>100</v>
       </c>
       <c r="E32" t="s">
         <v>80</v>
@@ -1313,8 +1313,8 @@
       <c r="C33" t="s">
         <v>68</v>
       </c>
-      <c r="D33" t="s">
-        <v>68</v>
+      <c r="D33">
+        <v>100</v>
       </c>
       <c r="E33" t="s">
         <v>80</v>
@@ -1333,8 +1333,8 @@
       <c r="C34" t="s">
         <v>73</v>
       </c>
-      <c r="D34" t="s">
-        <v>68</v>
+      <c r="D34">
+        <v>100</v>
       </c>
       <c r="E34" t="s">
         <v>80</v>
@@ -1353,8 +1353,8 @@
       <c r="C35" t="s">
         <v>68</v>
       </c>
-      <c r="D35" t="s">
-        <v>68</v>
+      <c r="D35">
+        <v>100</v>
       </c>
       <c r="E35" t="s">
         <v>80</v>
@@ -1373,8 +1373,8 @@
       <c r="C36" t="s">
         <v>70</v>
       </c>
-      <c r="D36" t="s">
-        <v>68</v>
+      <c r="D36">
+        <v>100</v>
       </c>
       <c r="E36" t="s">
         <v>81</v>
@@ -1393,8 +1393,8 @@
       <c r="C37" t="s">
         <v>70</v>
       </c>
-      <c r="D37" t="s">
-        <v>68</v>
+      <c r="D37">
+        <v>100</v>
       </c>
       <c r="E37" t="s">
         <v>68</v>
@@ -1413,8 +1413,8 @@
       <c r="C38" t="s">
         <v>76</v>
       </c>
-      <c r="D38" t="s">
-        <v>68</v>
+      <c r="D38">
+        <v>100</v>
       </c>
       <c r="E38" t="s">
         <v>81</v>
@@ -1433,8 +1433,8 @@
       <c r="C39" t="s">
         <v>68</v>
       </c>
-      <c r="D39" t="s">
-        <v>68</v>
+      <c r="D39">
+        <v>100</v>
       </c>
       <c r="E39" t="s">
         <v>81</v>
@@ -1453,8 +1453,8 @@
       <c r="C40" t="s">
         <v>69</v>
       </c>
-      <c r="D40" t="s">
-        <v>68</v>
+      <c r="D40">
+        <v>100</v>
       </c>
       <c r="E40" t="s">
         <v>69</v>
@@ -1473,8 +1473,8 @@
       <c r="C41" t="s">
         <v>69</v>
       </c>
-      <c r="D41" t="s">
-        <v>68</v>
+      <c r="D41">
+        <v>100</v>
       </c>
       <c r="E41" t="s">
         <v>80</v>
@@ -1493,8 +1493,8 @@
       <c r="C42" t="s">
         <v>69</v>
       </c>
-      <c r="D42" t="s">
-        <v>68</v>
+      <c r="D42">
+        <v>100</v>
       </c>
       <c r="E42" t="s">
         <v>81</v>
@@ -1513,8 +1513,8 @@
       <c r="C43" t="s">
         <v>73</v>
       </c>
-      <c r="D43" t="s">
-        <v>68</v>
+      <c r="D43">
+        <v>100</v>
       </c>
       <c r="E43" t="s">
         <v>80</v>
@@ -1533,8 +1533,8 @@
       <c r="C44" t="s">
         <v>73</v>
       </c>
-      <c r="D44" t="s">
-        <v>68</v>
+      <c r="D44">
+        <v>100</v>
       </c>
       <c r="E44" t="s">
         <v>80</v>
@@ -1553,8 +1553,8 @@
       <c r="C45" t="s">
         <v>70</v>
       </c>
-      <c r="D45" t="s">
-        <v>68</v>
+      <c r="D45">
+        <v>100</v>
       </c>
       <c r="E45" t="s">
         <v>80</v>
@@ -1573,8 +1573,8 @@
       <c r="C46" t="s">
         <v>70</v>
       </c>
-      <c r="D46" t="s">
-        <v>68</v>
+      <c r="D46">
+        <v>100</v>
       </c>
       <c r="E46" t="s">
         <v>80</v>
@@ -1593,8 +1593,8 @@
       <c r="C47" t="s">
         <v>68</v>
       </c>
-      <c r="D47" t="s">
-        <v>68</v>
+      <c r="D47">
+        <v>100</v>
       </c>
       <c r="E47" t="s">
         <v>80</v>
@@ -1613,8 +1613,8 @@
       <c r="C48" t="s">
         <v>68</v>
       </c>
-      <c r="D48" t="s">
-        <v>68</v>
+      <c r="D48">
+        <v>100</v>
       </c>
       <c r="E48" t="s">
         <v>81</v>
@@ -1633,8 +1633,8 @@
       <c r="C49" t="s">
         <v>77</v>
       </c>
-      <c r="D49" t="s">
-        <v>68</v>
+      <c r="D49">
+        <v>100</v>
       </c>
       <c r="E49" t="s">
         <v>80</v>
@@ -1653,8 +1653,8 @@
       <c r="C50" t="s">
         <v>68</v>
       </c>
-      <c r="D50" t="s">
-        <v>68</v>
+      <c r="D50">
+        <v>100</v>
       </c>
       <c r="E50" t="s">
         <v>82</v>
@@ -1673,8 +1673,8 @@
       <c r="C51" t="s">
         <v>78</v>
       </c>
-      <c r="D51" t="s">
-        <v>68</v>
+      <c r="D51">
+        <v>100</v>
       </c>
       <c r="E51" t="s">
         <v>80</v>
@@ -1693,8 +1693,8 @@
       <c r="C52" t="s">
         <v>69</v>
       </c>
-      <c r="D52" t="s">
-        <v>68</v>
+      <c r="D52">
+        <v>100</v>
       </c>
       <c r="E52" t="s">
         <v>69</v>
@@ -1713,8 +1713,8 @@
       <c r="C53" t="s">
         <v>74</v>
       </c>
-      <c r="D53" t="s">
-        <v>68</v>
+      <c r="D53">
+        <v>100</v>
       </c>
       <c r="E53" t="s">
         <v>68</v>
@@ -1733,8 +1733,8 @@
       <c r="C54" t="s">
         <v>69</v>
       </c>
-      <c r="D54" t="s">
-        <v>68</v>
+      <c r="D54">
+        <v>100</v>
       </c>
       <c r="E54" t="s">
         <v>69</v>
@@ -1753,8 +1753,8 @@
       <c r="C55" t="s">
         <v>69</v>
       </c>
-      <c r="D55" t="s">
-        <v>68</v>
+      <c r="D55">
+        <v>100</v>
       </c>
       <c r="E55" t="s">
         <v>69</v>
@@ -1773,8 +1773,8 @@
       <c r="C56" t="s">
         <v>79</v>
       </c>
-      <c r="D56" t="s">
-        <v>68</v>
+      <c r="D56">
+        <v>100</v>
       </c>
       <c r="E56" t="s">
         <v>68</v>

</xml_diff>